<commit_message>
Comments tab. Added value boxes.
</commit_message>
<xml_diff>
--- a/VOTOS + COMENTARIOS Cambio Climático.xlsx
+++ b/VOTOS + COMENTARIOS Cambio Climático.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/Congreso Virtual/Cambio Climático/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE559B9F-72EB-2946-ABCA-E88A8D587A11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BB423A-882C-944F-A249-A24DD4CA9210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VOTO GENERAL" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Key" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">COMENTARIOS!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">COMENTARIOS!$A$1:$F$30</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VOTO GENERAL'!$A$1:$U$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4594" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4603" uniqueCount="169">
   <si>
     <t xml:space="preserve">vote </t>
   </si>
@@ -547,6 +547,9 @@
   <si>
     <t xml:space="preserve">Plazo muy largo y objetivos insuficientes                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                        </t>
   </si>
+  <si>
+    <t>No responde</t>
+  </si>
 </sst>
 </file>
 
@@ -900,9 +903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A66BC0-2683-7241-8FC0-48B2AEE57E6D}">
   <dimension ref="A1:U260"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="R230" sqref="R230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17815,24 +17818,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D1D18F-2D82-624E-8780-7CF4C7DD4A5D}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="89" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="2" width="57.5" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27" style="5" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="4"/>
     <col min="4" max="4" width="13" style="4" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" style="4" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -17848,167 +17851,236 @@
       <c r="E1" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.2">
+      <c r="F1" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
+        <v>19245</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="272" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>19245</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>23445</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>27115</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>33825</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>51559</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="221" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>125151</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="4">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="289" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>61747</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>92140</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="4">
-        <v>3</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>117067</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="4">
-        <v>3</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>33825</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="4">
-        <v>2</v>
+      <c r="D7" s="4">
+        <v>0</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
+        <v>61747</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="170" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>70067</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>108505</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>134571</v>
+        <v>84113</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="C10" s="4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="404" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>137754</v>
+        <v>92131</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C11" s="4">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>92140</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>19245</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>27115</v>
+        <v>95209</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -18017,41 +18089,53 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>92131</v>
+        <v>108505</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>95209</v>
+        <v>110768</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>111746</v>
       </c>
@@ -18061,190 +18145,298 @@
       <c r="C16" s="4">
         <v>1</v>
       </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
       <c r="E16" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="272" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
+        <v>117067</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="4">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>125151</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="4">
+        <v>6</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="372" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>128847</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>163790</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="153" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>200086</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="C19" s="4">
         <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="F19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>203195</v>
+        <v>134571</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="404" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>203432</v>
+        <v>137754</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C21" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0</v>
       </c>
       <c r="E21" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>163790</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>203491</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
-        <v>203582</v>
+        <v>174774</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C23" s="4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="340" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
-        <v>84113</v>
+        <v>200086</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C24" s="4">
         <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="255" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
-        <v>19245</v>
+        <v>200750</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>157</v>
+        <v>160</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="289" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+      <c r="F25" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="306" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
-        <v>23445</v>
+        <v>203195</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>135</v>
+        <v>154</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="F26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="388" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
-        <v>110768</v>
+        <v>203432</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>158</v>
+        <v>138</v>
+      </c>
+      <c r="C27" s="4">
+        <v>1</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="F27" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
-        <v>174774</v>
+        <v>203452</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>159</v>
+        <v>161</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
-        <v>200750</v>
+        <v>203491</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
-        <v>203452</v>
+        <v>203582</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>161</v>
+        <v>167</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>163</v>
       </c>
+      <c r="F30" s="4" t="s">
+        <v>168</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{D68B5EFA-0FE2-1542-B714-105AC21E749A}"/>
+  <autoFilter ref="A1:F30" xr:uid="{316BF650-8745-7148-A2F6-60A1F0CCC60F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>